<commit_message>
feat: change rxnConfidenceScores to double
</commit_message>
<xml_diff>
--- a/readme/RAVEN_structure_fields.xlsx
+++ b/readme/RAVEN_structure_fields.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simmarc/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simmarc/Box Sync/3_functions/0_matlab/RAVEN/readme/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="27260" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="38400" windowHeight="20040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -479,7 +479,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -593,6 +593,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1425,7 +1428,7 @@
         <v>4</v>
       </c>
       <c r="D42" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E42" t="s">
         <v>75</v>

</xml_diff>

<commit_message>
feat: fix subSystems field
Fixed all the functions involving subSystems field. Also fixed KEGG, MetaCyc and HMR databases, since the Matlab structures with subSystems as cell array columns of string are no longer compatible with export functions.
</commit_message>
<xml_diff>
--- a/readme/RAVEN_structure_fields.xlsx
+++ b/readme/RAVEN_structure_fields.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="150">
   <si>
     <t>Description</t>
   </si>
@@ -236,9 +236,6 @@
     <t>Reaction compartments</t>
   </si>
   <si>
-    <t>Subsystem name for each reaction</t>
-  </si>
-  <si>
     <t>Reaction-to-gene mapping in sparse matrix form</t>
   </si>
   <si>
@@ -474,6 +471,12 @@
   </si>
   <si>
     <t>If missing during the model export, it is exported as blankName</t>
+  </si>
+  <si>
+    <t>Column Struct of Cell Array of Strings</t>
+  </si>
+  <si>
+    <t>Subsystem names for each reaction</t>
   </si>
 </sst>
 </file>
@@ -880,27 +883,27 @@
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="6"/>
       <c r="B1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7"/>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="8"/>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>1</v>
@@ -909,10 +912,10 @@
         <v>0</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -920,16 +923,16 @@
         <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E6" t="s">
         <v>53</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -937,16 +940,16 @@
         <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E7" t="s">
         <v>54</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -968,13 +971,13 @@
         <v>40</v>
       </c>
       <c r="E9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F9">
         <v>-1000</v>
       </c>
       <c r="G9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -985,13 +988,13 @@
         <v>40</v>
       </c>
       <c r="E10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F10">
         <v>1000</v>
       </c>
       <c r="G10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -999,13 +1002,13 @@
         <v>45</v>
       </c>
       <c r="D11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -1013,13 +1016,13 @@
         <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -1027,13 +1030,13 @@
         <v>47</v>
       </c>
       <c r="D13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -1041,13 +1044,13 @@
         <v>48</v>
       </c>
       <c r="D14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -1055,13 +1058,13 @@
         <v>49</v>
       </c>
       <c r="D15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1069,13 +1072,13 @@
         <v>50</v>
       </c>
       <c r="D16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.2">
@@ -1089,7 +1092,7 @@
         <v>56</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
@@ -1103,7 +1106,7 @@
         <v>57</v>
       </c>
       <c r="F18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.2">
@@ -1154,7 +1157,7 @@
         <v>39</v>
       </c>
       <c r="E22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F22">
         <v>1</v>
@@ -1193,7 +1196,7 @@
         <v>63</v>
       </c>
       <c r="F25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
@@ -1207,7 +1210,7 @@
         <v>64</v>
       </c>
       <c r="F26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.2">
@@ -1235,7 +1238,7 @@
         <v>66</v>
       </c>
       <c r="G28" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.2">
@@ -1246,10 +1249,10 @@
         <v>38</v>
       </c>
       <c r="E29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F29" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.2">
@@ -1260,10 +1263,10 @@
         <v>38</v>
       </c>
       <c r="E30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.2">
@@ -1277,7 +1280,7 @@
         <v>67</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.2">
@@ -1294,7 +1297,7 @@
         <v>1</v>
       </c>
       <c r="G32" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.2">
@@ -1305,10 +1308,10 @@
         <v>38</v>
       </c>
       <c r="E33" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.2">
@@ -1319,7 +1322,7 @@
         <v>37</v>
       </c>
       <c r="E34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.2">
@@ -1327,13 +1330,13 @@
         <v>13</v>
       </c>
       <c r="D35" t="s">
-        <v>38</v>
+        <v>148</v>
       </c>
       <c r="E35" t="s">
-        <v>69</v>
+        <v>149</v>
       </c>
       <c r="F35" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.2">
@@ -1344,10 +1347,10 @@
         <v>38</v>
       </c>
       <c r="E36" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.2">
@@ -1358,10 +1361,10 @@
         <v>41</v>
       </c>
       <c r="E37" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G37" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.2">
@@ -1372,10 +1375,10 @@
         <v>38</v>
       </c>
       <c r="E38" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.2">
@@ -1386,10 +1389,10 @@
         <v>38</v>
       </c>
       <c r="E39" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F39" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.2">
@@ -1400,10 +1403,10 @@
         <v>38</v>
       </c>
       <c r="E40" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F40" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.2">
@@ -1414,13 +1417,13 @@
         <v>38</v>
       </c>
       <c r="E41" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F41" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G41" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.2">
@@ -1431,7 +1434,7 @@
         <v>39</v>
       </c>
       <c r="E42" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F42">
         <v>3</v>
@@ -1445,7 +1448,7 @@
         <v>38</v>
       </c>
       <c r="E43" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.2">
@@ -1456,13 +1459,13 @@
         <v>38</v>
       </c>
       <c r="E44" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F44">
         <v>1</v>
       </c>
       <c r="G44" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.2">
@@ -1473,10 +1476,10 @@
         <v>41</v>
       </c>
       <c r="E45" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G45" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.2">
@@ -1487,10 +1490,10 @@
         <v>38</v>
       </c>
       <c r="E46" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F46" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.2">
@@ -1501,10 +1504,10 @@
         <v>38</v>
       </c>
       <c r="E47" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F47" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.2">
@@ -1515,10 +1518,10 @@
         <v>38</v>
       </c>
       <c r="E48" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.2">
@@ -1529,10 +1532,10 @@
         <v>38</v>
       </c>
       <c r="E49" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F49" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.2">
@@ -1543,13 +1546,13 @@
         <v>39</v>
       </c>
       <c r="E50" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F50">
         <v>1</v>
       </c>
       <c r="G50" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.2">
@@ -1560,10 +1563,10 @@
         <v>38</v>
       </c>
       <c r="E51" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F51" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.2">
@@ -1574,10 +1577,10 @@
         <v>38</v>
       </c>
       <c r="E52" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F52" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.2">
@@ -1588,10 +1591,10 @@
         <v>41</v>
       </c>
       <c r="E53" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G53" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.2">
@@ -1602,10 +1605,10 @@
         <v>38</v>
       </c>
       <c r="E54" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F54" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.2">
@@ -1616,10 +1619,10 @@
         <v>38</v>
       </c>
       <c r="E55" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F55" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.2">
@@ -1630,13 +1633,13 @@
         <v>39</v>
       </c>
       <c r="E56" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F56">
         <v>0</v>
       </c>
       <c r="G56" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.2">
@@ -1647,30 +1650,30 @@
         <v>39</v>
       </c>
       <c r="E57" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F57">
         <v>0</v>
       </c>
       <c r="G57" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B58" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D58" t="s">
         <v>38</v>
       </c>
       <c r="E58" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F58" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
style: excel MODEL tab
* changed order to have taxonomy in a more important position
* removed default options (unclear why were they needed to begin with)
</commit_message>
<xml_diff>
--- a/readme/RAVEN_structure_fields.xlsx
+++ b/readme/RAVEN_structure_fields.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simmarc/Box Sync/3_functions/0_matlab/RAVEN/readme/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bensan\Documents\repos\RAVEN\readme\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{98F3ABAA-24AC-43F9-90BF-7CDA212D84EB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="38400" windowHeight="20040" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="444" windowWidth="38400" windowHeight="20040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -389,9 +390,6 @@
     <t>The organization of the main model author</t>
   </si>
   <si>
-    <t>The taxonomy ID for the target species</t>
-  </si>
-  <si>
     <t>Additional comments about the model</t>
   </si>
   <si>
@@ -477,12 +475,15 @@
   </si>
   <si>
     <t>Subsystem names for each reaction</t>
+  </si>
+  <si>
+    <t>The taxonomy for the target species</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -866,39 +867,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="15.83203125" customWidth="1"/>
+    <col min="1" max="2" width="15.796875" customWidth="1"/>
     <col min="3" max="3" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="61.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="15.83203125" customWidth="1"/>
+    <col min="6" max="7" width="15.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="7"/>
       <c r="B2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="8"/>
       <c r="B3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="9" t="s">
         <v>105</v>
       </c>
@@ -912,13 +915,13 @@
         <v>0</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>21</v>
       </c>
@@ -932,10 +935,10 @@
         <v>86</v>
       </c>
       <c r="G6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>20</v>
       </c>
@@ -949,10 +952,10 @@
         <v>87</v>
       </c>
       <c r="G7" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>22</v>
       </c>
@@ -963,111 +966,111 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" t="s">
+        <v>112</v>
+      </c>
+      <c r="E9" t="s">
+        <v>149</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C10" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="D9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" t="s">
-        <v>114</v>
-      </c>
-      <c r="F9">
-        <v>-1000</v>
-      </c>
-      <c r="G9" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C10" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="D10" t="s">
         <v>40</v>
       </c>
       <c r="E10" t="s">
+        <v>114</v>
+      </c>
+      <c r="F10">
+        <v>-1000</v>
+      </c>
+      <c r="G10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" t="s">
         <v>115</v>
       </c>
-      <c r="F10">
+      <c r="F11">
         <v>1000</v>
       </c>
-      <c r="G10" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C11" s="1" t="s">
+      <c r="G11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C12" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="D11" t="s">
-        <v>112</v>
-      </c>
-      <c r="E11" t="s">
-        <v>117</v>
-      </c>
-      <c r="F11" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C12" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="D12" t="s">
         <v>112</v>
       </c>
       <c r="E12" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F12" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C13" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D13" t="s">
         <v>112</v>
       </c>
       <c r="E13" t="s">
-        <v>118</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="F13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C14" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D14" t="s">
         <v>112</v>
       </c>
       <c r="E14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C15" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D15" t="s">
         <v>112</v>
       </c>
       <c r="E15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C16" s="1" t="s">
         <v>50</v>
       </c>
@@ -1075,13 +1078,13 @@
         <v>112</v>
       </c>
       <c r="E16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>2</v>
       </c>
@@ -1092,10 +1095,10 @@
         <v>56</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>8</v>
       </c>
@@ -1109,7 +1112,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>14</v>
       </c>
@@ -1120,7 +1123,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>11</v>
       </c>
@@ -1134,7 +1137,7 @@
         <v>-1000</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
         <v>12</v>
       </c>
@@ -1148,7 +1151,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
         <v>17</v>
       </c>
@@ -1163,7 +1166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
         <v>16</v>
       </c>
@@ -1174,7 +1177,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B24" s="2" t="s">
         <v>15</v>
       </c>
@@ -1185,7 +1188,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
         <v>25</v>
       </c>
@@ -1199,7 +1202,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>26</v>
       </c>
@@ -1213,7 +1216,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>27</v>
       </c>
@@ -1227,7 +1230,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>28</v>
       </c>
@@ -1238,10 +1241,10 @@
         <v>66</v>
       </c>
       <c r="G28" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C29" s="1" t="s">
         <v>51</v>
       </c>
@@ -1255,7 +1258,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C30" s="1" t="s">
         <v>52</v>
       </c>
@@ -1269,7 +1272,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>3</v>
       </c>
@@ -1280,10 +1283,10 @@
         <v>67</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>34</v>
       </c>
@@ -1297,10 +1300,10 @@
         <v>1</v>
       </c>
       <c r="G32" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>19</v>
       </c>
@@ -1311,10 +1314,10 @@
         <v>109</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>7</v>
       </c>
@@ -1325,21 +1328,21 @@
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>13</v>
       </c>
       <c r="D35" t="s">
+        <v>147</v>
+      </c>
+      <c r="E35" t="s">
         <v>148</v>
-      </c>
-      <c r="E35" t="s">
-        <v>149</v>
       </c>
       <c r="F35" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>29</v>
       </c>
@@ -1353,7 +1356,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>30</v>
       </c>
@@ -1364,10 +1367,10 @@
         <v>71</v>
       </c>
       <c r="G37" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C38" s="1" t="s">
         <v>51</v>
       </c>
@@ -1381,7 +1384,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C39" s="1" t="s">
         <v>52</v>
       </c>
@@ -1395,7 +1398,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>6</v>
       </c>
@@ -1406,10 +1409,10 @@
         <v>72</v>
       </c>
       <c r="F40" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>5</v>
       </c>
@@ -1420,13 +1423,13 @@
         <v>73</v>
       </c>
       <c r="F41" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G41" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>4</v>
       </c>
@@ -1440,7 +1443,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>18</v>
       </c>
@@ -1451,7 +1454,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>35</v>
       </c>
@@ -1465,10 +1468,10 @@
         <v>1</v>
       </c>
       <c r="G44" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>31</v>
       </c>
@@ -1479,10 +1482,10 @@
         <v>77</v>
       </c>
       <c r="G45" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C46" s="1" t="s">
         <v>51</v>
       </c>
@@ -1493,10 +1496,10 @@
         <v>109</v>
       </c>
       <c r="F46" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C47" s="1" t="s">
         <v>52</v>
       </c>
@@ -1507,10 +1510,10 @@
         <v>110</v>
       </c>
       <c r="F47" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>42</v>
       </c>
@@ -1521,10 +1524,10 @@
         <v>78</v>
       </c>
       <c r="F48" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>9</v>
       </c>
@@ -1535,10 +1538,10 @@
         <v>79</v>
       </c>
       <c r="F49" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B50" s="2" t="s">
         <v>23</v>
       </c>
@@ -1552,10 +1555,10 @@
         <v>1</v>
       </c>
       <c r="G50" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>32</v>
       </c>
@@ -1566,10 +1569,10 @@
         <v>81</v>
       </c>
       <c r="F51" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>10</v>
       </c>
@@ -1580,10 +1583,10 @@
         <v>82</v>
       </c>
       <c r="F52" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>33</v>
       </c>
@@ -1594,10 +1597,10 @@
         <v>83</v>
       </c>
       <c r="G53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C54" s="1" t="s">
         <v>51</v>
       </c>
@@ -1608,10 +1611,10 @@
         <v>109</v>
       </c>
       <c r="F54" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C55" s="1" t="s">
         <v>52</v>
       </c>
@@ -1622,10 +1625,10 @@
         <v>110</v>
       </c>
       <c r="F55" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>36</v>
       </c>
@@ -1639,10 +1642,10 @@
         <v>0</v>
       </c>
       <c r="G56" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>24</v>
       </c>
@@ -1656,10 +1659,10 @@
         <v>0</v>
       </c>
       <c r="G57" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B58" s="12" t="s">
         <v>111</v>
       </c>
@@ -1667,16 +1670,17 @@
         <v>38</v>
       </c>
       <c r="E58" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F58" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G58" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>